<commit_message>
update 40x vplans interrupts, fencei, counters
Signed-off-by: Robin Pedersen <Robin.Pedersen@silabs.com>
</commit_message>
<xml_diff>
--- a/docs/VerifPlans/Simulation/micro_architecture/CV32E40X_fencei.xlsx
+++ b/docs/VerifPlans/Simulation/micro_architecture/CV32E40X_fencei.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ropeders\Documents\fencei_vplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C58AF8-9BA6-4863-91BD-C5D0D450F0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600DC2DB-04BA-4235-A9C1-BAF80C52A4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,26 +26,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={2F57A4C5-8706-4FC8-8CE8-0C6AADC484ED}</author>
-  </authors>
-  <commentList>
-    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{2F57A4C5-8706-4FC8-8CE8-0C6AADC484ED}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Or should this NOT be tried, because it is undefined behavior and because it will most likely conflict with the iss?</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="96">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -185,9 +167,6 @@
     <t>Ack change</t>
   </si>
   <si>
-    <t>Branch</t>
-  </si>
-  <si>
     <t>Flush</t>
   </si>
   <si>
@@ -197,9 +176,6 @@
     <t>Riscv spec</t>
   </si>
   <si>
-    <t>No guarantee</t>
-  </si>
-  <si>
     <t>Stores complete</t>
   </si>
   <si>
@@ -242,18 +218,12 @@
     <t>After a fence.i instruction has been executed, all preceding store instructions shall have their effects visible to the instruction fetch of the instructions that are to be executed after the fence.i instruction.</t>
   </si>
   <si>
-    <t>By default, RISC-V does not guarantee that stores will be visible to instruction fetches</t>
-  </si>
-  <si>
     <t>imm[11:0], rs1, rd are reserved for future extensions, and implementations shall ignore them</t>
   </si>
   <si>
     <t>Try giving random values in those fields and see that all else works as expected</t>
   </si>
   <si>
-    <t>Given zero stalls on neither instr-side and data-side obi nor on fencei_flush_ack_i, then the execution of fence.i takes 2 or 3 cycles</t>
-  </si>
-  <si>
     <t>Fill up the write buffer prior to executing a fence.i and ensure that fencei_flush_req_o holds off going high until the write buffer to has been emptied</t>
   </si>
   <si>
@@ -269,9 +239,6 @@
     <t>Drive ack to test all permutations of rising/falling before/after/on req, acking without req, retracting an early ack, delaying ack after req, etc.</t>
   </si>
   <si>
-    <t>Upon a req, try witholding ack for a long time and see that the fence.i can be stalled arbitrarily long</t>
-  </si>
-  <si>
     <t>Fetching</t>
   </si>
   <si>
@@ -284,21 +251,12 @@
     <t>Check that a fence.i will cause flushing of the pipeline, prefetcher, write buffer, and data_req_o</t>
   </si>
   <si>
-    <t>If possible, have the fence.i and the following instruction(s) be prefetched, but let the instruction right before the fence.i write a different instruction to the address following the fence.i, then observe that the written instruction is executed instead of the original one and that no side-effects (csr updates or otherwise) occur (can possibly mix 16bit/32bit instructions to force a noticable difference)</t>
-  </si>
-  <si>
     <t>Check that after having read one value from an address, then after storing a value to that same address, if executing that address then the value shall always be that which was written (should work well in both sim/formal)</t>
   </si>
   <si>
     <t>Make sure a store instruction is run right before a fence.i, and (possibly using obi stalls) ensure that the fence.i is pending retirement but holds off until the store's data_rvalid_i is clocked in and that fencei_flush_req_o was low until this point where it now goes high</t>
   </si>
   <si>
-    <t>Observe stores to the next PC, without any fence.i in between (any outcome is acceptable, but this should arguably still be tried in case there are any unforeseen problems with it)</t>
-  </si>
-  <si>
-    <t>Check that stores to the address of the instruction following a fence.i gets reflected in the execution of the instruction following the fence.i (the abstraction level of the ISS should make for a reliable comparison)</t>
-  </si>
-  <si>
     <t>Check that when executing a fence.i instruction there will be a rising req before has retired</t>
   </si>
   <si>
@@ -321,6 +279,42 @@
   </si>
   <si>
     <t>Check that all stores (either to next pc or other places) preceding a fence.i will complete on the bus (excluding exceptions/interrupts/etc) and be readable afterwards (particularly, ensure that the write buffer isn't just purged)</t>
+  </si>
+  <si>
+    <t>Branch initiated</t>
+  </si>
+  <si>
+    <t>Shadowing branch</t>
+  </si>
+  <si>
+    <t>Take a branch or do a jump to skip a fence.i, and ensure that fencei_flush_req_o doesn't go high</t>
+  </si>
+  <si>
+    <t>If the fence.i ends up not retiring because it was preceeded by a taken branch or a jump, then the fencei_flush_req_o shall not go high</t>
+  </si>
+  <si>
+    <t>Given zero stalls on neither instr-side and data-side obi nor on fencei_flush_ack_i, then the execution of fence.i takes 2 or 3 cycles (three when target is non-word-aligned non-RVC)</t>
+  </si>
+  <si>
+    <t>Upon a req, try witholding ack for a long time and see that the fence.i can be stalled arbitrarily long (should have covers for ack delays of at least {[0:5]})</t>
+  </si>
+  <si>
+    <t>Req wait OBI</t>
+  </si>
+  <si>
+    <t>fencei_flush_req_o shall not go high while there are outstanding stores on the obi bus</t>
+  </si>
+  <si>
+    <t>Check vs the OBI monitors that there are no outstanding stores at the time fencei_flush_req_o goes high</t>
+  </si>
+  <si>
+    <t>Do a fencei, but right before the fencei do a store to the instruction following the fencei, then see that the newly stored value is executed instead of the old instruction (e.g. change addi to use a different immediate)</t>
+  </si>
+  <si>
+    <t>Do a fencei and then some known instruction, but let the environment detect when the fencei is being executed and change the memory holding the next instruction, then see that the old instruction is not executed</t>
+  </si>
+  <si>
+    <t>Let the instruction right before a fence.i write a different instruction to the address following the fence.i, then observe that the written instruction is executed instead of the original one and that no side-effects (csr updates or otherwise) occur (can possibly mix 16bit/32bit instructions to force a noticable difference)</t>
   </si>
 </sst>
 </file>
@@ -522,9 +516,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Robin Pedersen" id="{3C0FA6B8-FDF8-4FDA-B4A9-EF789180BFC5}" userId="S::ropeders@silabs.com::adb93be4-7511-46a9-b0a0-7c4c8c1f1b0c" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -822,29 +814,21 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E18" dT="2021-09-21T11:02:44.84" personId="{3C0FA6B8-FDF8-4FDA-B4A9-EF789180BFC5}" id="{2F57A4C5-8706-4FC8-8CE8-0C6AADC484ED}">
-    <text>Or should this NOT be tried, because it is undefined behavior and because it will most likely conflict with the iss?</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMJ36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="51.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="41.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
@@ -884,19 +868,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>16</v>
@@ -909,59 +893,51 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" s="5" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="5" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>43</v>
-      </c>
+    <row r="5" spans="1:9" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>19</v>
@@ -974,7 +950,7 @@
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" s="5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>38</v>
       </c>
@@ -982,26 +958,26 @@
         <v>41</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>38</v>
       </c>
@@ -1009,13 +985,13 @@
         <v>41</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>85</v>
-      </c>
       <c r="E7" s="7" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>19</v>
@@ -1028,7 +1004,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>38</v>
       </c>
@@ -1036,13 +1012,13 @@
         <v>41</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>19</v>
@@ -1055,7 +1031,7 @@
       </c>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
@@ -1063,26 +1039,26 @@
         <v>41</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>38</v>
       </c>
@@ -1090,26 +1066,26 @@
         <v>41</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>38</v>
       </c>
@@ -1117,26 +1093,26 @@
         <v>41</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>26</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>38</v>
       </c>
@@ -1144,16 +1120,16 @@
         <v>41</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>26</v>
@@ -1168,14 +1144,16 @@
         <v>38</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="D13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>19</v>
@@ -1184,23 +1162,25 @@
         <v>26</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="D14" s="7" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>19</v>
@@ -1209,53 +1189,63 @@
         <v>26</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="7"/>
+        <v>41</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="D15" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
+    <row r="16" spans="1:9" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="D16" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="F16" s="7" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>38</v>
       </c>
@@ -1264,10 +1254,10 @@
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>19</v>
@@ -1280,82 +1270,96 @@
       </c>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+    <row r="18" spans="1:9" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>50</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>23</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>49</v>
+    <row r="20" spans="1:9" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="F20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G21" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="6"/>
-    </row>
-    <row r="21" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1501,26 +1505,36 @@
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
     </row>
-    <row r="35" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+    <row r="35" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="A36:I36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -1531,7 +1545,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>H2:H34</xm:sqref>
+          <xm:sqref>H2:H35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
@@ -1540,7 +1554,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>G2:G34</xm:sqref>
+          <xm:sqref>G2:G35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -1549,7 +1563,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>F2:F34</xm:sqref>
+          <xm:sqref>F2:F35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1738,13 +1752,13 @@
     </row>
     <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E6" s="14"/>
     </row>

</xml_diff>